<commit_message>
Added first deliverable hand in
</commit_message>
<xml_diff>
--- a/Project Management/Project Plan.xlsx
+++ b/Project Management/Project Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22266" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22266" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Design Program Structure and Features</t>
+  </si>
+  <si>
+    <t>Write Final Dissertation</t>
+  </si>
+  <si>
+    <t>First Deliverable submitted</t>
   </si>
 </sst>
 </file>
@@ -222,9 +228,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$24</c:f>
+              <c:f>Sheet1!$A$2:$B$26</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="25"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>First Deliverable</c:v>
@@ -236,63 +242,69 @@
                     <c:v>Ethics Form submitted</c:v>
                   </c:pt>
                   <c:pt idx="3">
+                    <c:v>First Deliverable submitted</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>Interview with Supervisor and Second Reader</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>Development of Package</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>Design Program Structure and Features</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>Implementation of Main Features</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>Develop Unit Tests</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>Documentation of Current Features</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="10">
                     <c:v>Implementation of Less Important Features</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="11">
                     <c:v>Develop Unit Tests for Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="12">
                     <c:v>Documentation of Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="13">
+                    <c:v>Write Final Dissertation</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Write Draft of Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="15">
                     <c:v>Draft Dissertation to Supervisor</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="16">
                     <c:v>Improve from feedback given</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="17">
                     <c:v>Dissertation submitted</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="18">
                     <c:v>Poster Deliverable</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="19">
                     <c:v>Poster Design</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="20">
                     <c:v>Create Poster</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="21">
                     <c:v>Send Poster for Printing</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="22">
                     <c:v>Prepare for Session</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="23">
                     <c:v>Poster Session</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="24">
                     <c:v>Poster Submitted</c:v>
                   </c:pt>
                 </c:lvl>
@@ -310,61 +322,67 @@
                     <c:v>4</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>5</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>6</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>7</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>8</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>9</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="10">
                     <c:v>10</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="11">
                     <c:v>11</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="12">
                     <c:v>12</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="13">
                     <c:v>13</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>14</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="15">
                     <c:v>15</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="16">
                     <c:v>16</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>17</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>18</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>19</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>20</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>21</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>22</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>23</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>24</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -372,10 +390,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$24</c:f>
+              <c:f>Sheet1!$C$2:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>43003</c:v>
                 </c:pt>
@@ -386,63 +404,69 @@
                   <c:v>43061</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>43065</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>43083</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43067</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>43067</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>43067</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>43076</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43111</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43114</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43117</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43121</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43124</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43127</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>43127</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>43170</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>43171</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>43212</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>43210</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>43210</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>43212</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="21">
                   <c:v>43215</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="22">
                   <c:v>43216</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>43223</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>43225</c:v>
                 </c:pt>
               </c:numCache>
@@ -470,7 +494,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="00B0F0"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -478,11 +502,72 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-F90E-4315-AF5F-52CFD52D47ED}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$24</c:f>
+              <c:f>Sheet1!$A$2:$B$26</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="25"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>First Deliverable</c:v>
@@ -494,63 +579,69 @@
                     <c:v>Ethics Form submitted</c:v>
                   </c:pt>
                   <c:pt idx="3">
+                    <c:v>First Deliverable submitted</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>Interview with Supervisor and Second Reader</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>Development of Package</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>Design Program Structure and Features</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>Implementation of Main Features</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>Develop Unit Tests</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>Documentation of Current Features</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="10">
                     <c:v>Implementation of Less Important Features</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="11">
                     <c:v>Develop Unit Tests for Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="12">
                     <c:v>Documentation of Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="13">
+                    <c:v>Write Final Dissertation</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Write Draft of Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="15">
                     <c:v>Draft Dissertation to Supervisor</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="16">
                     <c:v>Improve from feedback given</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="17">
                     <c:v>Dissertation submitted</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="18">
                     <c:v>Poster Deliverable</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="19">
                     <c:v>Poster Design</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="20">
                     <c:v>Create Poster</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="21">
                     <c:v>Send Poster for Printing</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="22">
                     <c:v>Prepare for Session</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="23">
                     <c:v>Poster Session</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="24">
                     <c:v>Poster Submitted</c:v>
                   </c:pt>
                 </c:lvl>
@@ -568,61 +659,67 @@
                     <c:v>4</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>5</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>6</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="7">
                     <c:v>7</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="8">
                     <c:v>8</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>9</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="10">
                     <c:v>10</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="11">
                     <c:v>11</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="12">
                     <c:v>12</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="13">
                     <c:v>13</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>14</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="15">
                     <c:v>15</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="16">
                     <c:v>16</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>17</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>18</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>19</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>20</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>21</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>22</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>23</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>24</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -630,10 +727,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$24</c:f>
+              <c:f>Sheet1!$E$2:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>63</c:v>
                 </c:pt>
@@ -647,60 +744,66 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="20">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -750,7 +853,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -813,7 +916,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="t" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1445,10 +1548,10 @@
       <xdr:rowOff>163902</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>172528</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>172530</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>353683</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>43132</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1741,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1803,7 +1906,7 @@
         <v>43059</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E24" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E26" si="0">D3-C3</f>
         <v>1</v>
       </c>
     </row>
@@ -1825,18 +1928,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1">
-        <v>43083</v>
+        <v>43065</v>
       </c>
       <c r="D5" s="1">
-        <v>43084</v>
+        <v>43066</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
@@ -1845,88 +1948,88 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1">
-        <v>43067</v>
+        <v>43083</v>
       </c>
       <c r="D6" s="1">
-        <v>43126</v>
+        <v>43084</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>43067</v>
       </c>
       <c r="D7" s="1">
-        <v>43075</v>
+        <v>43126</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
-        <v>43076</v>
+        <v>43067</v>
       </c>
       <c r="D8" s="1">
-        <v>43110</v>
+        <v>43075</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1">
-        <v>43111</v>
+        <v>43076</v>
       </c>
       <c r="D9" s="1">
-        <v>43113</v>
+        <v>43110</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
-        <v>43114</v>
+        <v>43111</v>
       </c>
       <c r="D10" s="1">
-        <v>43116</v>
+        <v>43113</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
@@ -1935,124 +2038,124 @@
     </row>
     <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
-        <v>43117</v>
+        <v>43114</v>
       </c>
       <c r="D11" s="1">
-        <v>43120</v>
+        <v>43116</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1">
-        <v>43121</v>
+        <v>43117</v>
       </c>
       <c r="D12" s="1">
-        <v>43123</v>
+        <v>43120</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1">
-        <v>43124</v>
+        <v>43121</v>
       </c>
       <c r="D13" s="1">
-        <v>43126</v>
+        <v>43123</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
-        <v>43127</v>
+        <v>43124</v>
       </c>
       <c r="D14" s="1">
-        <v>43170</v>
+        <v>43126</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1">
-        <v>43170</v>
+        <v>43127</v>
       </c>
       <c r="D15" s="1">
-        <v>43171</v>
+        <v>43213</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1">
-        <v>43171</v>
+        <v>43127</v>
       </c>
       <c r="D16" s="1">
-        <v>43212</v>
+        <v>43170</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>43212</v>
+        <v>43170</v>
       </c>
       <c r="D17" s="1">
-        <v>43213</v>
+        <v>43171</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
@@ -2061,106 +2164,106 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C18" s="1">
-        <v>43210</v>
+        <v>43171</v>
       </c>
       <c r="D18" s="1">
-        <v>43227</v>
+        <v>43212</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C19" s="1">
-        <v>43210</v>
+        <v>43212</v>
       </c>
       <c r="D19" s="1">
-        <v>43212</v>
+        <v>43213</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1">
-        <v>43212</v>
+        <v>43210</v>
       </c>
       <c r="D20" s="1">
-        <v>43215</v>
+        <v>43227</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1">
-        <v>43215</v>
+        <v>43210</v>
       </c>
       <c r="D21" s="1">
-        <v>43216</v>
+        <v>43212</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1">
-        <v>43216</v>
+        <v>43212</v>
       </c>
       <c r="D22" s="1">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1">
-        <v>43223</v>
+        <v>43215</v>
       </c>
       <c r="D23" s="1">
-        <v>43224</v>
+        <v>43216</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
@@ -2169,18 +2272,54 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1">
+        <v>43216</v>
+      </c>
+      <c r="D24" s="1">
+        <v>43223</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43223</v>
+      </c>
+      <c r="D25" s="1">
+        <v>43224</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C26" s="1">
         <v>43225</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D26" s="1">
         <v>43227</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E26" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2195,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6E260C-CEE2-4450-A8DB-52D8BA7888C4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Made the changes Michael mentioned in todays meeting
Changed the colouring of the bars in the chart
Added in a task for improving software after feedback
Adjusted software development times
Removed operators section from section 4
</commit_message>
<xml_diff>
--- a/Project Management/Project Plan.xlsx
+++ b/Project Management/Project Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22266" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22266" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>First Deliverable submitted</t>
+  </si>
+  <si>
+    <t>Improve Package from feedback</t>
+  </si>
+  <si>
+    <t>Develop Unit Tests for New Features</t>
+  </si>
+  <si>
+    <t>Documentation of New Features</t>
   </si>
 </sst>
 </file>
@@ -228,9 +237,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$26</c:f>
+              <c:f>Sheet1!$A$2:$B$29</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>First Deliverable</c:v>
@@ -266,45 +275,54 @@
                     <c:v>Implementation of Less Important Features</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Develop Unit Tests for New Features</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Documentation of New Features</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Improve Package from feedback</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Develop Unit Tests for Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>Documentation of Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>Write Final Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>Write Draft of Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="18">
                     <c:v>Draft Dissertation to Supervisor</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="19">
                     <c:v>Improve from feedback given</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="20">
                     <c:v>Dissertation submitted</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="21">
                     <c:v>Poster Deliverable</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="22">
                     <c:v>Poster Design</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="23">
                     <c:v>Create Poster</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="24">
                     <c:v>Send Poster for Printing</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="25">
                     <c:v>Prepare for Session</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="26">
                     <c:v>Poster Session</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="27">
                     <c:v>Poster Submitted</c:v>
                   </c:pt>
                 </c:lvl>
@@ -322,67 +340,76 @@
                     <c:v>4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4</c:v>
+                    <c:v>5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>5</c:v>
+                    <c:v>6</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>6</c:v>
+                    <c:v>7</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>7</c:v>
+                    <c:v>8</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>8</c:v>
+                    <c:v>9</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>9</c:v>
+                    <c:v>10</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>10</c:v>
+                    <c:v>11</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>11</c:v>
+                    <c:v>12</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>12</c:v>
+                    <c:v>13</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>13</c:v>
+                    <c:v>14</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>14</c:v>
+                    <c:v>15</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>15</c:v>
+                    <c:v>16</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>16</c:v>
+                    <c:v>17</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>17</c:v>
+                    <c:v>18</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>18</c:v>
+                    <c:v>19</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>19</c:v>
+                    <c:v>20</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>20</c:v>
+                    <c:v>21</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>21</c:v>
+                    <c:v>22</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>22</c:v>
+                    <c:v>23</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>23</c:v>
+                    <c:v>24</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>24</c:v>
+                    <c:v>25</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>26</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>27</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>28</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -390,10 +417,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$26</c:f>
+              <c:f>Sheet1!$C$2:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>43003</c:v>
                 </c:pt>
@@ -416,13 +443,13 @@
                   <c:v>43067</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43076</c:v>
+                  <c:v>43075</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43111</c:v>
+                  <c:v>43110</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43114</c:v>
+                  <c:v>43113</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>43117</c:v>
@@ -431,43 +458,52 @@
                   <c:v>43121</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43124</c:v>
+                  <c:v>43123</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43127</c:v>
+                  <c:v>43126</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43127</c:v>
+                  <c:v>43130</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43136</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43136</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>43170</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>43171</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43212</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43210</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43210</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>43212</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>43210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43210</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43212</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>43215</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>43216</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>43223</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>43225</c:v>
+                <c:pt idx="27">
+                  <c:v>43224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -508,7 +544,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -527,7 +563,26 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3071-4329-8EAC-74FEC9C2668E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -536,26 +591,12 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="13"/>
+            <c:idx val="21"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="18"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -565,9 +606,9 @@
           </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$26</c:f>
+              <c:f>Sheet1!$A$2:$B$29</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>First Deliverable</c:v>
@@ -603,45 +644,54 @@
                     <c:v>Implementation of Less Important Features</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Develop Unit Tests for New Features</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Documentation of New Features</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Improve Package from feedback</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
                     <c:v>Develop Unit Tests for Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>Documentation of Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>Write Final Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>Write Draft of Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="18">
                     <c:v>Draft Dissertation to Supervisor</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="19">
                     <c:v>Improve from feedback given</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="20">
                     <c:v>Dissertation submitted</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="21">
                     <c:v>Poster Deliverable</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="22">
                     <c:v>Poster Design</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="23">
                     <c:v>Create Poster</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="24">
                     <c:v>Send Poster for Printing</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="25">
                     <c:v>Prepare for Session</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="26">
                     <c:v>Poster Session</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="27">
                     <c:v>Poster Submitted</c:v>
                   </c:pt>
                 </c:lvl>
@@ -659,67 +709,76 @@
                     <c:v>4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4</c:v>
+                    <c:v>5</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>5</c:v>
+                    <c:v>6</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>6</c:v>
+                    <c:v>7</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>7</c:v>
+                    <c:v>8</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>8</c:v>
+                    <c:v>9</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>9</c:v>
+                    <c:v>10</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>10</c:v>
+                    <c:v>11</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>11</c:v>
+                    <c:v>12</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>12</c:v>
+                    <c:v>13</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>13</c:v>
+                    <c:v>14</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>14</c:v>
+                    <c:v>15</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>15</c:v>
+                    <c:v>16</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>16</c:v>
+                    <c:v>17</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>17</c:v>
+                    <c:v>18</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>18</c:v>
+                    <c:v>19</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>19</c:v>
+                    <c:v>20</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>20</c:v>
+                    <c:v>21</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>21</c:v>
+                    <c:v>22</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>22</c:v>
+                    <c:v>23</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>23</c:v>
+                    <c:v>24</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>24</c:v>
+                    <c:v>25</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>26</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>27</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>28</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -727,10 +786,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$26</c:f>
+              <c:f>Sheet1!$E$2:$E$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>63</c:v>
                 </c:pt>
@@ -747,19 +806,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3</c:v>
@@ -768,43 +827,52 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43</c:v>
-                </c:pt>
                 <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>2</c:v>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1844,10 +1912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1974,7 @@
         <v>43059</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E26" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E29" si="0">D3-C3</f>
         <v>1</v>
       </c>
     </row>
@@ -1948,7 +2016,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>18</v>
@@ -1966,7 +2034,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
@@ -1975,16 +2043,16 @@
         <v>43067</v>
       </c>
       <c r="D7" s="1">
-        <v>43126</v>
+        <v>43136</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>27</v>
@@ -2002,61 +2070,61 @@
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="1">
-        <v>43076</v>
+        <v>43075</v>
       </c>
       <c r="D9" s="1">
         <v>43110</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="1">
-        <v>43111</v>
+        <v>43110</v>
       </c>
       <c r="D10" s="1">
         <v>43113</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="1">
-        <v>43114</v>
+        <v>43113</v>
       </c>
       <c r="D11" s="1">
-        <v>43116</v>
+        <v>43117</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>22</v>
@@ -2074,10 +2142,10 @@
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1">
         <v>43121</v>
@@ -2092,236 +2160,290 @@
     </row>
     <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1">
-        <v>43124</v>
+        <v>43123</v>
       </c>
       <c r="D14" s="1">
         <v>43126</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43126</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43130</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43130</v>
+      </c>
+      <c r="D16" s="1">
+        <v>43132</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43132</v>
+      </c>
+      <c r="D17" s="1">
+        <v>43136</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="1">
-        <v>43127</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C18" s="1">
+        <v>43136</v>
+      </c>
+      <c r="D18" s="1">
         <v>43213</v>
       </c>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="1">
-        <v>43127</v>
-      </c>
-      <c r="D16" s="1">
-        <v>43170</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1">
-        <v>43170</v>
-      </c>
-      <c r="D17" s="1">
-        <v>43171</v>
-      </c>
-      <c r="E17" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1">
-        <v>43171</v>
-      </c>
-      <c r="D18" s="1">
-        <v>43212</v>
-      </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1">
-        <v>43212</v>
+        <v>43136</v>
       </c>
       <c r="D19" s="1">
-        <v>43213</v>
+        <v>43170</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="C20" s="1">
-        <v>43210</v>
+        <v>43170</v>
       </c>
       <c r="D20" s="1">
-        <v>43227</v>
+        <v>43171</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C21" s="1">
-        <v>43210</v>
+        <v>43171</v>
       </c>
       <c r="D21" s="1">
         <v>43212</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C22" s="1">
         <v>43212</v>
       </c>
       <c r="D22" s="1">
-        <v>43215</v>
+        <v>43213</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C23" s="1">
-        <v>43215</v>
+        <v>43210</v>
       </c>
       <c r="D23" s="1">
-        <v>43216</v>
+        <v>43227</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1">
-        <v>43216</v>
+        <v>43210</v>
       </c>
       <c r="D24" s="1">
-        <v>43223</v>
+        <v>43212</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1">
-        <v>43223</v>
+        <v>43212</v>
       </c>
       <c r="D25" s="1">
-        <v>43224</v>
+        <v>43215</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1">
+        <v>43215</v>
+      </c>
+      <c r="D26" s="1">
+        <v>43216</v>
+      </c>
+      <c r="E26" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="1">
+        <v>43216</v>
+      </c>
+      <c r="D27" s="1">
+        <v>43223</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C26" s="1">
-        <v>43225</v>
-      </c>
-      <c r="D26" s="1">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1">
+        <v>43223</v>
+      </c>
+      <c r="D28" s="1">
+        <v>43224</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43224</v>
+      </c>
+      <c r="D29" s="1">
         <v>43227</v>
       </c>
-      <c r="E26" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="E29" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2334,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6E260C-CEE2-4450-A8DB-52D8BA7888C4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z30" sqref="Z30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Made changes that michael suggested
Still have to update the CGP packages section and possibly the
requirements
</commit_message>
<xml_diff>
--- a/Project Management/Project Plan.xlsx
+++ b/Project Management/Project Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22266" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22266" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -79,15 +79,9 @@
     <t>Interview with Supervisor and Second Reader</t>
   </si>
   <si>
-    <t>Develop Unit Tests</t>
-  </si>
-  <si>
     <t>Implementation of Main Features</t>
   </si>
   <si>
-    <t>Documentation of Current Features</t>
-  </si>
-  <si>
     <t>Implementation of Less Important Features</t>
   </si>
   <si>
@@ -112,13 +106,22 @@
     <t>First Deliverable submitted</t>
   </si>
   <si>
-    <t>Improve Package from feedback</t>
-  </si>
-  <si>
-    <t>Develop Unit Tests for New Features</t>
-  </si>
-  <si>
-    <t>Documentation of New Features</t>
+    <t>Carry out first User Study</t>
+  </si>
+  <si>
+    <t>Refine Requirements</t>
+  </si>
+  <si>
+    <t>Carry out final User Study</t>
+  </si>
+  <si>
+    <t>Implementation of New Main Features</t>
+  </si>
+  <si>
+    <t>Documentation of Main Features</t>
+  </si>
+  <si>
+    <t>Develop Unit Tests for Main Features</t>
   </si>
 </sst>
 </file>
@@ -134,12 +137,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -154,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -165,6 +180,8 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,9 +254,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$29</c:f>
+              <c:f>Sheet1!$A$2:$B$30</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>First Deliverable</c:v>
@@ -266,63 +283,66 @@
                     <c:v>Implementation of Main Features</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Develop Unit Tests</c:v>
+                    <c:v>Develop Unit Tests for Main Features</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Documentation of Current Features</c:v>
+                    <c:v>Documentation of Main Features</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Carry out first User Study</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Refine Requirements</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Implementation of New Main Features</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>Implementation of Less Important Features</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Develop Unit Tests for New Features</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Documentation of New Features</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Improve Package from feedback</c:v>
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>Develop Unit Tests for Final Version</c:v>
                   </c:pt>
                   <c:pt idx="15">
+                    <c:v>Carry out final User Study</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>Documentation of Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>Write Final Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>Write Draft of Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>Draft Dissertation to Supervisor</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>Improve from feedback given</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>Dissertation submitted</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>Poster Deliverable</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>Poster Design</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="24">
                     <c:v>Create Poster</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="25">
                     <c:v>Send Poster for Printing</c:v>
                   </c:pt>
-                  <c:pt idx="25">
+                  <c:pt idx="26">
                     <c:v>Prepare for Session</c:v>
                   </c:pt>
-                  <c:pt idx="26">
+                  <c:pt idx="27">
                     <c:v>Poster Session</c:v>
                   </c:pt>
-                  <c:pt idx="27">
+                  <c:pt idx="28">
                     <c:v>Poster Submitted</c:v>
                   </c:pt>
                 </c:lvl>
@@ -410,6 +430,9 @@
                   </c:pt>
                   <c:pt idx="27">
                     <c:v>28</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>29</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -417,10 +440,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$29</c:f>
+              <c:f>Sheet1!$C$2:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm\-yy</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>43003</c:v>
                 </c:pt>
@@ -437,72 +460,75 @@
                   <c:v>43083</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43067</c:v>
+                  <c:v>43066</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43067</c:v>
+                  <c:v>43066</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>43075</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43110</c:v>
+                  <c:v>43105</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43113</c:v>
+                  <c:v>43109</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>43114</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>43117</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>43121</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>43123</c:v>
+                  <c:v>43119</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43126</c:v>
+                  <c:v>43130</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43130</c:v>
+                  <c:v>43137</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43132</c:v>
+                  <c:v>43141</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43136</c:v>
+                  <c:v>43144</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43136</c:v>
+                  <c:v>43150</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>43150</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>43170</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>43171</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>43212</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43210</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>43210</c:v>
                 </c:pt>
                 <c:pt idx="23">
+                  <c:v>43210</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>43212</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>43215</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>43216</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>43223</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>43224</c:v>
                 </c:pt>
               </c:numCache>
@@ -577,7 +603,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="16"/>
+            <c:idx val="17"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -591,7 +617,7 @@
             </c:spPr>
           </c:dPt>
           <c:dPt>
-            <c:idx val="21"/>
+            <c:idx val="22"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -606,9 +632,9 @@
           </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$29</c:f>
+              <c:f>Sheet1!$A$2:$B$30</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>First Deliverable</c:v>
@@ -635,63 +661,66 @@
                     <c:v>Implementation of Main Features</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Develop Unit Tests</c:v>
+                    <c:v>Develop Unit Tests for Main Features</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Documentation of Current Features</c:v>
+                    <c:v>Documentation of Main Features</c:v>
                   </c:pt>
                   <c:pt idx="10">
+                    <c:v>Carry out first User Study</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Refine Requirements</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Implementation of New Main Features</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>Implementation of Less Important Features</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>Develop Unit Tests for New Features</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Documentation of New Features</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>Improve Package from feedback</c:v>
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>Develop Unit Tests for Final Version</c:v>
                   </c:pt>
                   <c:pt idx="15">
+                    <c:v>Carry out final User Study</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>Documentation of Final Version</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>Write Final Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>Write Draft of Dissertation</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>Draft Dissertation to Supervisor</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>Improve from feedback given</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>Dissertation submitted</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>Poster Deliverable</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>Poster Design</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="24">
                     <c:v>Create Poster</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="25">
                     <c:v>Send Poster for Printing</c:v>
                   </c:pt>
-                  <c:pt idx="25">
+                  <c:pt idx="26">
                     <c:v>Prepare for Session</c:v>
                   </c:pt>
-                  <c:pt idx="26">
+                  <c:pt idx="27">
                     <c:v>Poster Session</c:v>
                   </c:pt>
-                  <c:pt idx="27">
+                  <c:pt idx="28">
                     <c:v>Poster Submitted</c:v>
                   </c:pt>
                 </c:lvl>
@@ -779,6 +808,9 @@
                   </c:pt>
                   <c:pt idx="27">
                     <c:v>28</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>29</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -786,10 +818,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$29</c:f>
+              <c:f>Sheet1!$E$2:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>63</c:v>
                 </c:pt>
@@ -806,19 +838,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3</c:v>
@@ -827,51 +859,54 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -1912,10 +1947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="A1:D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1925,9 +1960,9 @@
     <col min="3" max="4" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1942,8 +1977,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1960,8 +1995,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1974,12 +2009,12 @@
         <v>43059</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E29" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E30" si="0">D3-C3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1996,12 +2031,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
         <v>43065</v>
@@ -2014,8 +2049,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -2032,416 +2067,443 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="1">
-        <v>43067</v>
+        <f>D2</f>
+        <v>43066</v>
       </c>
       <c r="D7" s="1">
-        <v>43136</v>
+        <f>MAX(D8:D18)</f>
+        <v>43150</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1">
-        <v>43067</v>
+        <f>D2</f>
+        <v>43066</v>
       </c>
       <c r="D8" s="1">
         <v>43075</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1">
         <v>43075</v>
       </c>
       <c r="D9" s="1">
-        <v>43110</v>
+        <v>43105</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43105</v>
+      </c>
+      <c r="D10" s="1">
+        <v>43109</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43109</v>
+      </c>
+      <c r="D11" s="1">
+        <v>43114</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1">
+        <v>43114</v>
+      </c>
+      <c r="D12" s="1">
+        <v>43117</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43117</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43119</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43119</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43130</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43130</v>
+      </c>
+      <c r="D15" s="1">
+        <v>43137</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43137</v>
+      </c>
+      <c r="D16" s="1">
+        <v>43141</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43141</v>
+      </c>
+      <c r="D17" s="1">
+        <v>43144</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43144</v>
+      </c>
+      <c r="D18" s="1">
+        <v>43150</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1">
+        <f>D7</f>
+        <v>43150</v>
+      </c>
+      <c r="D19" s="1">
+        <f>MAX(D20:D23)</f>
+        <v>43213</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="C10" s="1">
-        <v>43110</v>
-      </c>
-      <c r="D10" s="1">
-        <v>43113</v>
-      </c>
-      <c r="E10" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="B20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1">
+        <f>C19</f>
+        <v>43150</v>
+      </c>
+      <c r="D20" s="1">
+        <v>43170</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43170</v>
+      </c>
+      <c r="D21" s="1">
+        <v>43171</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="C11" s="1">
-        <v>43113</v>
-      </c>
-      <c r="D11" s="1">
-        <v>43117</v>
-      </c>
-      <c r="E11" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="B22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1">
+        <v>43171</v>
+      </c>
+      <c r="D22" s="1">
+        <v>43212</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="C12" s="1">
-        <v>43117</v>
-      </c>
-      <c r="D12" s="1">
-        <v>43120</v>
-      </c>
-      <c r="E12" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="1">
-        <v>43121</v>
-      </c>
-      <c r="D13" s="1">
-        <v>43123</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="1">
-        <v>43123</v>
-      </c>
-      <c r="D14" s="1">
-        <v>43126</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1">
-        <v>43126</v>
-      </c>
-      <c r="D15" s="1">
-        <v>43130</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="B23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1">
+        <v>43212</v>
+      </c>
+      <c r="D23" s="1">
+        <v>43213</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="C16" s="1">
-        <v>43130</v>
-      </c>
-      <c r="D16" s="1">
-        <v>43132</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1">
-        <v>43132</v>
-      </c>
-      <c r="D17" s="1">
-        <v>43136</v>
-      </c>
-      <c r="E17" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="1">
-        <v>43136</v>
-      </c>
-      <c r="D18" s="1">
-        <v>43213</v>
-      </c>
-      <c r="E18" s="4">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1">
-        <v>43136</v>
-      </c>
-      <c r="D19" s="1">
-        <v>43170</v>
-      </c>
-      <c r="E19" s="4">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="1">
-        <v>43170</v>
-      </c>
-      <c r="D20" s="1">
-        <v>43171</v>
-      </c>
-      <c r="E20" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="1">
-        <v>43171</v>
-      </c>
-      <c r="D21" s="1">
-        <v>43212</v>
-      </c>
-      <c r="E21" s="4">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1">
-        <v>43212</v>
-      </c>
-      <c r="D22" s="1">
-        <v>43213</v>
-      </c>
-      <c r="E22" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>9</v>
-      </c>
-      <c r="C23" s="1">
-        <v>43210</v>
-      </c>
-      <c r="D23" s="1">
-        <v>43227</v>
-      </c>
-      <c r="E23" s="4">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>10</v>
       </c>
       <c r="C24" s="1">
         <v>43210</v>
       </c>
       <c r="D24" s="1">
+        <v>43227</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1">
+        <v>43210</v>
+      </c>
+      <c r="D25" s="1">
         <v>43212</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E25" s="4">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <v>43212</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D26" s="1">
         <v>43215</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E26" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C27" s="1">
         <v>43215</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D27" s="1">
         <v>43216</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E27" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C28" s="1">
         <v>43216</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D28" s="1">
         <v>43223</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E28" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C29" s="1">
         <v>43223</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D29" s="1">
         <v>43224</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E29" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C30" s="1">
         <v>43224</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D30" s="1">
         <v>43227</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E30" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -2456,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6E260C-CEE2-4450-A8DB-52D8BA7888C4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z30" sqref="Z30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>